<commit_message>
added comment for mV@0A
</commit_message>
<xml_diff>
--- a/wiki/Other/openXvario Current Sensors.xlsx
+++ b/wiki/Other/openXvario Current Sensors.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rainer\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\openxvario\wiki\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="0" windowWidth="12885" windowHeight="6105"/>
+    <workbookView xWindow="2340" yWindow="0" windowWidth="12885" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Current Sensors for openXvario +C</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>example bidirectional Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ^ this value is normally OK for symetrical bidirectional sensors. For unidirectional sensors overwrite this formula with the mV the sensors puts out at 5V supply voltage and with 0A current</t>
   </si>
 </sst>
 </file>
@@ -155,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,8 +207,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -237,54 +246,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -293,17 +287,48 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -584,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,358 +621,389 @@
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="0.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="61.5" x14ac:dyDescent="0.9">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A2" s="18"/>
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="30" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="30"/>
-    </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="11"/>
-      <c r="B3" s="17" t="s">
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="7"/>
+      <c r="B3" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="15" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="15"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="9" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="18" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="20">
         <v>-100</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="J4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="27"/>
+      <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="10">
         <v>-5</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="10">
         <v>5</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="10">
         <v>185</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="8">
         <f>5000/(ABS(B6)+ABS(C6))*ABS(B6)</f>
         <v>2500</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <f>E6/D6*1000*-1</f>
         <v>-13513.513513513513</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <f>ABS((5000-E6)/D6*1000*-1)</f>
         <v>13513.513513513513</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="9">
         <f>F6+$I$4</f>
         <v>-13613.513513513513</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="9">
         <f>G6+$I$4</f>
         <v>13413.513513513513</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="10">
         <v>-20</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="10">
         <v>20</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="10">
         <v>100</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="8">
         <f t="shared" ref="E7:E9" si="0">5000/(ABS(B7)+ABS(C7))*ABS(B7)</f>
         <v>2500</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <f t="shared" ref="F7:F9" si="1">E7/D7*1000*-1</f>
         <v>-25000</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <f t="shared" ref="G7:G9" si="2">ABS((5000-E7)/D7*1000*-1)</f>
         <v>25000</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="9">
         <f t="shared" ref="H7:H9" si="3">F7+$I$4</f>
         <v>-25100</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="9">
         <f t="shared" ref="I7:I9" si="4">G7+$I$4</f>
         <v>24900</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="10">
         <v>-30</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="10">
         <v>30</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="10">
         <v>66</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <f t="shared" si="1"/>
         <v>-37878.787878787873</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="6">
         <f t="shared" si="2"/>
         <v>37878.787878787873</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="9">
         <f t="shared" si="3"/>
         <v>-37978.787878787873</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="9">
         <f t="shared" si="4"/>
         <v>37778.787878787873</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="10">
         <v>0</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="10">
         <v>30</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="10">
         <v>120</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <f t="shared" si="2"/>
         <v>41666.666666666664</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="9">
         <f t="shared" si="3"/>
         <v>-100</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="9">
         <f t="shared" si="4"/>
         <v>41566.666666666664</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="14">
         <v>-100</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="14">
         <v>100</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="14">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="13">
         <f t="shared" ref="E10" si="5">5000/(ABS(B10)+ABS(C10))*ABS(B10)</f>
         <v>2500</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="15">
         <f t="shared" ref="F10" si="6">E10/D10*1000*-1</f>
         <v>-125000</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="15">
         <f t="shared" ref="G10" si="7">ABS((5000-E10)/D10*1000*-1)</f>
         <v>125000</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="16">
         <f t="shared" ref="H10" si="8">F10+$I$4</f>
         <v>-125100</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="16">
         <f t="shared" ref="I10" si="9">G10+$I$4</f>
         <v>124900</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="14">
         <v>0</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="14">
         <v>125</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="14">
         <v>28</v>
       </c>
-      <c r="E11" s="21">
-        <f t="shared" ref="E11" si="10">5000/(ABS(B11)+ABS(C11))*ABS(B11)</f>
+      <c r="E11" s="13">
+        <f t="shared" ref="E11:E12" si="10">5000/(ABS(B11)+ABS(C11))*ABS(B11)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="15">
         <f t="shared" ref="F11" si="11">E11/D11*1000*-1</f>
         <v>0</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="15">
         <f t="shared" ref="G11" si="12">ABS((5000-E11)/D11*1000*-1)</f>
         <v>178571.42857142858</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="16">
         <f t="shared" ref="H11" si="13">F11+$I$4</f>
         <v>-100</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="16">
         <f t="shared" ref="I11" si="14">G11+$I$4</f>
         <v>178471.42857142858</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="28">
-        <v>0</v>
-      </c>
-      <c r="C12" s="28">
-        <v>125</v>
-      </c>
-      <c r="D12" s="28">
-        <v>28</v>
-      </c>
-      <c r="E12" s="12">
-        <f t="shared" ref="E12" si="15">5000/(ABS(B12)+ABS(C12))*ABS(B12)</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="8">
-        <f t="shared" ref="F12" si="16">E12/D12*1000*-1</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="8">
-        <f t="shared" ref="G12" si="17">ABS((5000-E12)/D12*1000*-1)</f>
-        <v>178571.42857142858</v>
-      </c>
-      <c r="H12" s="13">
-        <f t="shared" ref="H12" si="18">F12+$I$4</f>
-        <v>-100</v>
-      </c>
-      <c r="I12" s="13">
-        <f t="shared" ref="I12" si="19">G12+$I$4</f>
-        <v>178471.42857142858</v>
-      </c>
+      <c r="B12" s="19">
+        <v>30</v>
+      </c>
+      <c r="C12" s="19">
+        <v>30</v>
+      </c>
+      <c r="D12" s="19">
+        <v>66</v>
+      </c>
+      <c r="E12" s="34">
+        <f t="shared" si="10"/>
+        <v>2500</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" ref="F12" si="15">E12/D12*1000*-1</f>
+        <v>-37878.787878787873</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" ref="G12" si="16">ABS((5000-E12)/D12*1000*-1)</f>
+        <v>37878.787878787873</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" ref="H12" si="17">F12+$I$4</f>
+        <v>-37978.787878787873</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" ref="I12" si="18">G12+$I$4</f>
+        <v>37778.787878787873</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E13" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="32"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="E13:F19"/>
     <mergeCell ref="J4:L6"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:D2"/>

</xml_diff>

<commit_message>
fixed wrong column headers
</commit_message>
<xml_diff>
--- a/wiki/Other/openXvario Current Sensors.xlsx
+++ b/wiki/Other/openXvario Current Sensors.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="0" windowWidth="12885" windowHeight="6105"/>
+    <workbookView xWindow="7020" yWindow="0" windowWidth="12885" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Current Sensors for openXvario +C</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Start values</t>
   </si>
   <si>
-    <t>exampl unidirectional Sensor</t>
-  </si>
-  <si>
     <t>Sensor Module Parameters</t>
   </si>
   <si>
@@ -99,13 +96,34 @@
   </si>
   <si>
     <t xml:space="preserve"> ^ this value is normally OK for symetrical bidirectional sensors. For unidirectional sensors overwrite this formula with the mV the sensors puts out at 5V supply voltage and with 0A current</t>
+  </si>
+  <si>
+    <t>example unidirectional Sensor</t>
+  </si>
+  <si>
+    <t>mv@0A</t>
+  </si>
+  <si>
+    <t>mv/A</t>
+  </si>
+  <si>
+    <t>MaxCurrentMilliamps</t>
+  </si>
+  <si>
+    <t>ACS715ELCTR-20A-T</t>
+  </si>
+  <si>
+    <t>ACS715ELCTR-30A-T</t>
+  </si>
+  <si>
+    <t>ACS715LLCTR-20A-T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +171,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -256,10 +282,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -289,6 +316,28 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -322,15 +371,9 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,83 +667,92 @@
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20" style="1" customWidth="1"/>
+    <col min="10" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="61.5" x14ac:dyDescent="0.9">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A2" s="18"/>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="23" t="s">
+      <c r="G2" s="31"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24" t="s">
+      <c r="K2" s="32"/>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="7"/>
+      <c r="B3" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="38"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="38"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="37"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="20">
+        <v>-20</v>
+      </c>
+      <c r="L4" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="24"/>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="7"/>
-      <c r="B3" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="30"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="20">
-        <v>-100</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-    </row>
-    <row r="5" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+    </row>
+    <row r="5" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -713,24 +765,30 @@
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -755,19 +813,27 @@
         <f>ABS((5000-E6)/D6*1000*-1)</f>
         <v>13513.513513513513</v>
       </c>
-      <c r="H6" s="9">
-        <f>F6+$I$4</f>
-        <v>-13613.513513513513</v>
-      </c>
-      <c r="I6" s="9">
-        <f>G6+$I$4</f>
-        <v>13413.513513513513</v>
-      </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6" s="6">
+        <f t="shared" ref="H6:H16" si="0">5000/((G6-F6)/1000)</f>
+        <v>185</v>
+      </c>
+      <c r="I6" s="6">
+        <f>ABS(F6)/1000*D6</f>
+        <v>2500</v>
+      </c>
+      <c r="J6" s="9">
+        <f>F6+$K$4</f>
+        <v>-13533.513513513513</v>
+      </c>
+      <c r="K6" s="9">
+        <f>G6+$K$4</f>
+        <v>13493.513513513513</v>
+      </c>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
@@ -781,27 +847,35 @@
         <v>100</v>
       </c>
       <c r="E7" s="8">
-        <f t="shared" ref="E7:E9" si="0">5000/(ABS(B7)+ABS(C7))*ABS(B7)</f>
+        <f t="shared" ref="E7:E13" si="1">5000/(ABS(B7)+ABS(C7))*ABS(B7)</f>
         <v>2500</v>
       </c>
       <c r="F7" s="6">
-        <f t="shared" ref="F7:F9" si="1">E7/D7*1000*-1</f>
+        <f t="shared" ref="F7:F13" si="2">E7/D7*1000*-1</f>
         <v>-25000</v>
       </c>
       <c r="G7" s="6">
-        <f t="shared" ref="G7:G9" si="2">ABS((5000-E7)/D7*1000*-1)</f>
+        <f t="shared" ref="G7:G13" si="3">ABS((5000-E7)/D7*1000*-1)</f>
         <v>25000</v>
       </c>
-      <c r="H7" s="9">
-        <f t="shared" ref="H7:H9" si="3">F7+$I$4</f>
-        <v>-25100</v>
-      </c>
-      <c r="I7" s="9">
-        <f t="shared" ref="I7:I9" si="4">G7+$I$4</f>
-        <v>24900</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" s="6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" ref="I7:I16" si="4">ABS(F7)/1000*D7</f>
+        <v>2500</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" ref="J7:J13" si="5">F7+$K$4</f>
+        <v>-25020</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" ref="K7:K13" si="6">G7+$K$4</f>
+        <v>24980</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -815,208 +889,338 @@
         <v>66</v>
       </c>
       <c r="E8" s="8">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="2"/>
+        <v>-37878.787878787873</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="3"/>
+        <v>37878.787878787873</v>
+      </c>
+      <c r="H8" s="6">
         <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="4"/>
         <v>2500</v>
       </c>
-      <c r="F8" s="6">
+      <c r="J8" s="9">
+        <f t="shared" si="5"/>
+        <v>-37898.787878787873</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="6"/>
+        <v>37858.787878787873</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>20</v>
+      </c>
+      <c r="D9" s="10">
+        <v>185</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10">
+        <v>30</v>
+      </c>
+      <c r="D10" s="10">
+        <v>133</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10">
+        <v>185</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10">
+        <v>30</v>
+      </c>
+      <c r="D12" s="10">
+        <v>133</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>30</v>
+      </c>
+      <c r="D13" s="10">
+        <v>120</v>
+      </c>
+      <c r="E13" s="8">
         <f t="shared" si="1"/>
-        <v>-37878.787878787873</v>
-      </c>
-      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
         <f t="shared" si="2"/>
-        <v>37878.787878787873</v>
-      </c>
-      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
         <f t="shared" si="3"/>
-        <v>-37978.787878787873</v>
-      </c>
-      <c r="I8" s="9">
+        <v>41666.666666666664</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="I13" s="6">
         <f t="shared" si="4"/>
-        <v>37778.787878787873</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="10">
-        <v>30</v>
-      </c>
-      <c r="D9" s="10">
-        <v>120</v>
-      </c>
-      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="5"/>
+        <v>-20</v>
+      </c>
+      <c r="K13" s="9">
+        <f t="shared" si="6"/>
+        <v>41646.666666666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="14">
+        <v>-100</v>
+      </c>
+      <c r="C14" s="14">
+        <v>100</v>
+      </c>
+      <c r="D14" s="14">
+        <v>20</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" ref="E14" si="7">5000/(ABS(B14)+ABS(C14))*ABS(B14)</f>
+        <v>2500</v>
+      </c>
+      <c r="F14" s="15">
+        <f t="shared" ref="F14" si="8">E14/D14*1000*-1</f>
+        <v>-125000</v>
+      </c>
+      <c r="G14" s="15">
+        <f t="shared" ref="G14" si="9">ABS((5000-E14)/D14*1000*-1)</f>
+        <v>125000</v>
+      </c>
+      <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <f t="shared" si="2"/>
-        <v>41666.666666666664</v>
-      </c>
-      <c r="H9" s="9">
-        <f t="shared" si="3"/>
-        <v>-100</v>
-      </c>
-      <c r="I9" s="9">
+        <v>20</v>
+      </c>
+      <c r="I14" s="6">
         <f t="shared" si="4"/>
-        <v>41566.666666666664</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+        <v>2500</v>
+      </c>
+      <c r="J14" s="16">
+        <f t="shared" ref="J14" si="10">F14+$K$4</f>
+        <v>-125020</v>
+      </c>
+      <c r="K14" s="16">
+        <f t="shared" ref="K14" si="11">G14+$K$4</f>
+        <v>124980</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0</v>
+      </c>
+      <c r="C15" s="14">
+        <v>125</v>
+      </c>
+      <c r="D15" s="14">
+        <v>28</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" ref="E15" si="12">5000/(ABS(B15)+ABS(C15))*ABS(B15)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="15">
+        <f t="shared" ref="F15" si="13">E15/D15*1000*-1</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="15">
+        <f t="shared" ref="G15" si="14">ABS((5000-E15)/D15*1000*-1)</f>
+        <v>178571.42857142858</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="0"/>
+        <v>27.999999999999996</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="16">
+        <f t="shared" ref="J15" si="15">F15+$K$4</f>
+        <v>-20</v>
+      </c>
+      <c r="K15" s="16">
+        <f t="shared" ref="K15" si="16">G15+$K$4</f>
+        <v>178551.42857142858</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="19">
+        <v>0</v>
+      </c>
+      <c r="C16" s="19">
+        <v>100</v>
+      </c>
+      <c r="D16" s="19">
+        <v>40</v>
+      </c>
+      <c r="E16" s="21">
+        <v>600</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" ref="F16" si="17">E16/D16*1000*-1</f>
+        <v>-15000</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" ref="G16" si="18">ABS((5000-E16)/D16*1000*-1)</f>
+        <v>110000</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="4"/>
+        <v>600</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" ref="J16" si="19">F16+$K$4</f>
+        <v>-15020</v>
+      </c>
+      <c r="K16" s="9">
+        <f t="shared" ref="K16" si="20">G16+$K$4</f>
+        <v>109980</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E17" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="14">
-        <v>-100</v>
-      </c>
-      <c r="C10" s="14">
-        <v>100</v>
-      </c>
-      <c r="D10" s="14">
-        <v>20</v>
-      </c>
-      <c r="E10" s="13">
-        <f t="shared" ref="E10" si="5">5000/(ABS(B10)+ABS(C10))*ABS(B10)</f>
-        <v>2500</v>
-      </c>
-      <c r="F10" s="15">
-        <f t="shared" ref="F10" si="6">E10/D10*1000*-1</f>
-        <v>-125000</v>
-      </c>
-      <c r="G10" s="15">
-        <f t="shared" ref="G10" si="7">ABS((5000-E10)/D10*1000*-1)</f>
-        <v>125000</v>
-      </c>
-      <c r="H10" s="16">
-        <f t="shared" ref="H10" si="8">F10+$I$4</f>
-        <v>-125100</v>
-      </c>
-      <c r="I10" s="16">
-        <f t="shared" ref="I10" si="9">G10+$I$4</f>
-        <v>124900</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0</v>
-      </c>
-      <c r="C11" s="14">
-        <v>125</v>
-      </c>
-      <c r="D11" s="14">
-        <v>28</v>
-      </c>
-      <c r="E11" s="13">
-        <f t="shared" ref="E11:E12" si="10">5000/(ABS(B11)+ABS(C11))*ABS(B11)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="15">
-        <f t="shared" ref="F11" si="11">E11/D11*1000*-1</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="15">
-        <f t="shared" ref="G11" si="12">ABS((5000-E11)/D11*1000*-1)</f>
-        <v>178571.42857142858</v>
-      </c>
-      <c r="H11" s="16">
-        <f t="shared" ref="H11" si="13">F11+$I$4</f>
-        <v>-100</v>
-      </c>
-      <c r="I11" s="16">
-        <f t="shared" ref="I11" si="14">G11+$I$4</f>
-        <v>178471.42857142858</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="19">
-        <v>30</v>
-      </c>
-      <c r="C12" s="19">
-        <v>30</v>
-      </c>
-      <c r="D12" s="19">
-        <v>66</v>
-      </c>
-      <c r="E12" s="34">
-        <f t="shared" si="10"/>
-        <v>2500</v>
-      </c>
-      <c r="F12" s="6">
-        <f t="shared" ref="F12" si="15">E12/D12*1000*-1</f>
-        <v>-37878.787878787873</v>
-      </c>
-      <c r="G12" s="6">
-        <f t="shared" ref="G12" si="16">ABS((5000-E12)/D12*1000*-1)</f>
-        <v>37878.787878787873</v>
-      </c>
-      <c r="H12" s="9">
-        <f t="shared" ref="H12" si="17">F12+$I$4</f>
-        <v>-37978.787878787873</v>
-      </c>
-      <c r="I12" s="9">
-        <f t="shared" ref="I12" si="18">G12+$I$4</f>
-        <v>37778.787878787873</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="32"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
+      <c r="F17" s="27"/>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="J21">
+        <f>F15*D15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="E13:F19"/>
-    <mergeCell ref="J4:L6"/>
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="E17:F23"/>
+    <mergeCell ref="L4:N6"/>
+    <mergeCell ref="A1:K1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>